<commit_message>
Added pan check for all tests
</commit_message>
<xml_diff>
--- a/public/sample_uploads/co_invest_portfolio_investments_failed.xlsx
+++ b/public/sample_uploads/co_invest_portfolio_investments_failed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1867E7D-23EA-4E60-A521-98EFDBA565B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1959EB7C-35DF-44B5-8833-A7E9C1B999C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Portfolio Company Name *</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Domestic</t>
+  </si>
+  <si>
+    <t>Pan *</t>
+  </si>
+  <si>
+    <t>BUHNXDFEA7</t>
   </si>
 </sst>
 </file>
@@ -415,21 +421,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1328125" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -437,118 +444,127 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
         <v>44197</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2000000</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>20000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1">
         <v>44197</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1000000</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-12000</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>8</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed caching and archived migrations
</commit_message>
<xml_diff>
--- a/public/sample_uploads/co_invest_portfolio_investments_failed.xlsx
+++ b/public/sample_uploads/co_invest_portfolio_investments_failed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1959EB7C-35DF-44B5-8833-A7E9C1B999C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE2F545-4E16-401D-986B-71CF800ADD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Portfolio Company Name *</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>BUHNXDFEA7</t>
+  </si>
+  <si>
+    <t>Tech</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -511,6 +514,9 @@
       <c r="I2" t="s">
         <v>13</v>
       </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
       <c r="L2" t="s">
         <v>21</v>
       </c>
@@ -554,6 +560,9 @@
       </c>
       <c r="J3" t="s">
         <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
       </c>
       <c r="L3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Removed investor creation in PI and valuations import
</commit_message>
<xml_diff>
--- a/public/sample_uploads/co_invest_portfolio_investments_failed.xlsx
+++ b/public/sample_uploads/co_invest_portfolio_investments_failed.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA418FB6-A4FD-475F-A7E5-E6189B11B2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E31BA3-E44D-4205-A332-D2037D877115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Portfolio Company Name *</t>
   </si>
@@ -99,37 +99,17 @@
     <t>Domestic</t>
   </si>
   <si>
-    <t>BUHNXDFEA7</t>
-  </si>
-  <si>
     <t>Tech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pan </t>
-  </si>
-  <si>
-    <t>Primary Email *</t>
-  </si>
-  <si>
-    <t>tc@apple.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,17 +132,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,22 +418,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="22.1328125" customWidth="1"/>
-    <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -464,146 +440,128 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1">
+        <v>44197</v>
+      </c>
+      <c r="D2">
+        <v>2000000</v>
+      </c>
+      <c r="E2">
+        <v>20000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1">
-        <v>44197</v>
-      </c>
-      <c r="F2">
-        <v>2000000</v>
-      </c>
-      <c r="G2">
-        <v>20000</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1">
+        <v>44197</v>
+      </c>
+      <c r="D3">
+        <v>1000000</v>
+      </c>
+      <c r="E3">
+        <v>-12000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="1">
-        <v>44197</v>
-      </c>
-      <c r="F3">
-        <v>1000000</v>
-      </c>
-      <c r="G3">
-        <v>-12000</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{1E374C88-AA6A-4E5A-BE94-B5DB54BFBFAF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored portfolio to use instrument
</commit_message>
<xml_diff>
--- a/public/sample_uploads/co_invest_portfolio_investments_failed.xlsx
+++ b/public/sample_uploads/co_invest_portfolio_investments_failed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E31BA3-E44D-4205-A332-D2037D877115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7FF64E-0D6D-41F7-8CF6-65BCE7D54DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Portfolio Company Name *</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Tech</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Stock</t>
   </si>
 </sst>
 </file>
@@ -418,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -432,7 +438,7 @@
     <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -461,22 +467,25 @@
         <v>12</v>
       </c>
       <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -502,22 +511,25 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -546,18 +558,21 @@
         <v>15</v>
       </c>
       <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>8</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>